<commit_message>
some light ups for action collisions
</commit_message>
<xml_diff>
--- a/backend/jupyter/volume_sections/SHOOTING_COEF.xlsx
+++ b/backend/jupyter/volume_sections/SHOOTING_COEF.xlsx
@@ -453,609 +453,609 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>GK_y</t>
+          <t>GK_x</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.2962691765858401</v>
+        <v>0.2123405037926963</v>
       </c>
       <c r="C2" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2962691765858401</v>
+        <v>0.2123405037926963</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>tpr_y</t>
+          <t>tpr_x</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1650638234649887</v>
+        <v>0.01272532166281927</v>
       </c>
       <c r="C3" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1650638234649887</v>
+        <v>0.01272532166281927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Anticipation_y</t>
+          <t>Anticipation_x</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03044822662906781</v>
+        <v>0.012991908494656</v>
       </c>
       <c r="C4" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03044822662906781</v>
+        <v>0.012991908494656</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Teamwork_y</t>
+          <t>Teamwork_x</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.05016441879259161</v>
+        <v>0.06608506427750496</v>
       </c>
       <c r="C5" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05016441879259161</v>
+        <v>0.06608506427750496</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Corners_y</t>
+          <t>Corners_x</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1481832610314556</v>
+        <v>0.04236803143712155</v>
       </c>
       <c r="C6" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1481832610314556</v>
+        <v>0.04236803143712155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Dribbling_y</t>
+          <t>Dribbling_x</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.1460119810284922</v>
+        <v>-0.05819302642662285</v>
       </c>
       <c r="C7" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1460119810284922</v>
+        <v>0.05819302642662285</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Agility_y</t>
+          <t>Agility_x</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.1306632016633711</v>
+        <v>0.01822184493229715</v>
       </c>
       <c r="C8" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1306632016633711</v>
+        <v>0.01822184493229715</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Off_the_Ball_y</t>
+          <t>Off_the_Ball_x</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.007416350086683212</v>
+        <v>0.09703207705940729</v>
       </c>
       <c r="C9" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D9" t="n">
-        <v>0.007416350086683212</v>
+        <v>0.09703207705940729</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Penalty_Taking_y</t>
+          <t>Penalty_Taking_x</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.004950185399798432</v>
+        <v>0.01252964211970782</v>
       </c>
       <c r="C10" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D10" t="n">
-        <v>0.004950185399798432</v>
+        <v>0.01252964211970782</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Vision_y</t>
+          <t>Vision_x</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3454832229083359</v>
+        <v>-0.1809495666157287</v>
       </c>
       <c r="C11" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3454832229083359</v>
+        <v>0.1809495666157287</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Positioning_y</t>
+          <t>Positioning_x</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.03518900375106877</v>
+        <v>-0.03290121837836091</v>
       </c>
       <c r="C12" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03518900375106877</v>
+        <v>0.03290121837836091</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Acceleration_y</t>
+          <t>Acceleration_x</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.09466292023940986</v>
+        <v>0.07208681128406398</v>
       </c>
       <c r="C13" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D13" t="n">
-        <v>0.09466292023940986</v>
+        <v>0.07208681128406398</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Concentration_y</t>
+          <t>Concentration_x</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0511998473988779</v>
+        <v>-0.04060840441440411</v>
       </c>
       <c r="C14" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0511998473988779</v>
+        <v>0.04060840441440411</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Pace_y</t>
+          <t>Pace_x</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.03862642001162523</v>
+        <v>0.08911375318663163</v>
       </c>
       <c r="C15" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03862642001162523</v>
+        <v>0.08911375318663163</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Stamina_y</t>
+          <t>Stamina_x</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.05841876056114164</v>
+        <v>0.184177793245315</v>
       </c>
       <c r="C16" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05841876056114164</v>
+        <v>0.184177793245315</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Balance_y</t>
+          <t>Balance_x</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.09304894384358026</v>
+        <v>0.05727095918597623</v>
       </c>
       <c r="C17" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D17" t="n">
-        <v>0.09304894384358026</v>
+        <v>0.05727095918597623</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Flair_y</t>
+          <t>Flair_x</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.004553902714535263</v>
+        <v>-0.09380265541293856</v>
       </c>
       <c r="C18" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004553902714535263</v>
+        <v>0.09380265541293856</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Free_Kick_Taking_y</t>
+          <t>Free_Kick_Taking_x</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.06311024095132368</v>
+        <v>-0.009089981759475611</v>
       </c>
       <c r="C19" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D19" t="n">
-        <v>0.06311024095132368</v>
+        <v>0.009089981759475611</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Crossing_y</t>
+          <t>Crossing_x</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.148487525964312</v>
+        <v>0.129305608390409</v>
       </c>
       <c r="C20" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D20" t="n">
-        <v>0.148487525964312</v>
+        <v>0.129305608390409</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Jumping_Reach_y</t>
+          <t>Jumping_Reach_x</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.07554294157210301</v>
+        <v>-0.05762949200016387</v>
       </c>
       <c r="C21" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D21" t="n">
-        <v>0.07554294157210301</v>
+        <v>0.05762949200016387</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Natural_Fitness_y</t>
+          <t>Natural_Fitness_x</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.1401848004175587</v>
+        <v>-0.1045181032440784</v>
       </c>
       <c r="C22" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1401848004175587</v>
+        <v>0.1045181032440784</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Technique_y</t>
+          <t>Technique_x</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.1038150535384997</v>
+        <v>0.186089290247479</v>
       </c>
       <c r="C23" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1038150535384997</v>
+        <v>0.186089290247479</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Long_Throws_y</t>
+          <t>Long_Throws_x</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01715498605286207</v>
+        <v>0.09615381609156798</v>
       </c>
       <c r="C24" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01715498605286207</v>
+        <v>0.09615381609156798</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Strength_y</t>
+          <t>Strength_x</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.03665226625954602</v>
+        <v>-0.2017506910783503</v>
       </c>
       <c r="C25" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03665226625954602</v>
+        <v>0.2017506910783503</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Long_Shots_y</t>
+          <t>Long_Shots_x</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.1809656597276904</v>
+        <v>0.1569422774424056</v>
       </c>
       <c r="C26" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1809656597276904</v>
+        <v>0.1569422774424056</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Bravery_y</t>
+          <t>Bravery_x</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.03056333561394816</v>
+        <v>0.05242678821507071</v>
       </c>
       <c r="C27" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D27" t="n">
-        <v>0.03056333561394816</v>
+        <v>0.05242678821507071</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Finishing_y</t>
+          <t>Finishing_x</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.125935100496052</v>
+        <v>0.0875766324796652</v>
       </c>
       <c r="C28" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D28" t="n">
-        <v>0.125935100496052</v>
+        <v>0.0875766324796652</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Aggression_y</t>
+          <t>Aggression_x</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.08161826053922404</v>
+        <v>-0.09513435537874448</v>
       </c>
       <c r="C29" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D29" t="n">
-        <v>0.08161826053922404</v>
+        <v>0.09513435537874448</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Work_Rate_y</t>
+          <t>Work_Rate_x</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.002951439098743742</v>
+        <v>0.0341836388601659</v>
       </c>
       <c r="C30" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D30" t="n">
-        <v>0.002951439098743742</v>
+        <v>0.0341836388601659</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Heading_y</t>
+          <t>Heading_x</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.007728322700149955</v>
+        <v>0.1155589284683455</v>
       </c>
       <c r="C31" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D31" t="n">
-        <v>0.007728322700149955</v>
+        <v>0.1155589284683455</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Decisions_y</t>
+          <t>Decisions_x</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.1750889602678169</v>
+        <v>-0.07593378896341374</v>
       </c>
       <c r="C32" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1750889602678169</v>
+        <v>0.07593378896341374</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Tackling_y</t>
+          <t>Tackling_x</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.02176215753033925</v>
+        <v>0.05956084540852848</v>
       </c>
       <c r="C33" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02176215753033925</v>
+        <v>0.05956084540852848</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Marking_y</t>
+          <t>Marking_x</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.1036660013275758</v>
+        <v>-0.2329563806298866</v>
       </c>
       <c r="C34" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1036660013275758</v>
+        <v>0.2329563806298866</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Leadership_y</t>
+          <t>Leadership_x</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1411436598810174</v>
+        <v>0.02938124037041185</v>
       </c>
       <c r="C35" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1411436598810174</v>
+        <v>0.02938124037041185</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Composure_y</t>
+          <t>Composure_x</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.002566749458428051</v>
+        <v>-0.08052109668232832</v>
       </c>
       <c r="C36" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D36" t="n">
-        <v>0.002566749458428051</v>
+        <v>0.08052109668232832</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Determination_y</t>
+          <t>Determination_x</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.02442380261602556</v>
+        <v>-0.0830455389444307</v>
       </c>
       <c r="C37" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D37" t="n">
-        <v>0.02442380261602556</v>
+        <v>0.0830455389444307</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Passing_y</t>
+          <t>Passing_x</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.05514076008455829</v>
+        <v>-0.1423590412775249</v>
       </c>
       <c r="C38" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D38" t="n">
-        <v>0.05514076008455829</v>
+        <v>0.1423590412775249</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>First_Touch_y</t>
+          <t>First_Touch_x</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.0853992913253156</v>
+        <v>0.1059821678746613</v>
       </c>
       <c r="C39" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0853992913253156</v>
+        <v>0.1059821678746613</v>
       </c>
     </row>
     <row r="40">
@@ -1065,13 +1065,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.1848576279843757</v>
+        <v>0.01272532166281879</v>
       </c>
       <c r="C40" t="n">
-        <v>22.31238921520658</v>
+        <v>-16.59701423989972</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1848576279843757</v>
+        <v>0.01272532166281879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>